<commit_message>
fix bet target remvoe star mark many simulation
</commit_message>
<xml_diff>
--- a/resources/data_summary.xlsx
+++ b/resources/data_summary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="223">
   <si>
     <t>항목</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -778,6 +778,14 @@
   </si>
   <si>
     <t>부담중량 증감 / 공백출전일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마필가격</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연대점수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -836,7 +844,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -864,6 +872,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -900,7 +914,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -953,6 +967,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2052,7 +2069,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2205,7 +2222,7 @@
       <c r="F7" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="10" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2228,7 +2245,7 @@
       <c r="F8" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="10" t="s">
         <v>217</v>
       </c>
     </row>
@@ -2251,7 +2268,7 @@
       <c r="F9" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="10" t="s">
         <v>220</v>
       </c>
     </row>
@@ -2274,7 +2291,7 @@
       <c r="F10" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="10" t="s">
         <v>219</v>
       </c>
     </row>
@@ -2297,7 +2314,7 @@
       <c r="F11" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="10" t="s">
         <v>218</v>
       </c>
     </row>
@@ -2317,6 +2334,9 @@
       <c r="F12" s="12" t="s">
         <v>209</v>
       </c>
+      <c r="G12" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="10" t="s">
@@ -2330,6 +2350,9 @@
       </c>
       <c r="F13" s="12" t="s">
         <v>210</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">

</xml_diff>